<commit_message>
XGBoost Third model, extra features
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\quora-nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D240E171-EC77-4666-93B5-44398B8804B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E36B555-C2E3-4E6C-9B4C-585CC994E808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>Model</t>
   </si>
@@ -55,10 +55,6 @@
   </si>
   <si>
     <t>colsample_bytree': 0.7, 'learning_rate': np.float64(0.16737697032078552), 'max_depth': 9, 
-'min_child_weight': 5, 'n_estimators': 100, 'subsample': 0.9</t>
-  </si>
-  <si>
-    <t>colsample_bytree': 0.7, 'learning_rate': np.float64(0.16737697032078552), 'max_depth': 9, 
 'min_child_weight': 5, 'n_estimators': 100, 'subsample': 0.10</t>
   </si>
   <si>
@@ -134,6 +130,18 @@
   </si>
   <si>
     <t>Despite expectations, model underperformed</t>
+  </si>
+  <si>
+    <t>XGBoost + "all-mpnet-base-v2" BERT-Sentence Embedding</t>
+  </si>
+  <si>
+    <t>lowercase,
+punctuation removal
+extra features
+no stemming</t>
+  </si>
+  <si>
+    <t>colsample_bytree': 0.8, 'learning_rate': np.float64(0.03686562370169114), 'max_depth': 7, 'min_child_weight': 3, 'n_estimators': 200, 'subsample': 0.7</t>
   </si>
 </sst>
 </file>
@@ -575,7 +583,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -625,15 +633,15 @@
         <v>7</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="3">
         <v>0.44658444507828499</v>
@@ -642,27 +650,27 @@
         <v>0.78426377105542999</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3">
-        <v>0.32041683916555402</v>
+        <v>0.30713916629328603</v>
       </c>
       <c r="D4" s="3">
-        <v>0.852308986123822</v>
+        <v>0.86075589304707001</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -670,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>0.32041683916555402</v>
@@ -687,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>0.32041683916555402</v>
@@ -704,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>0.32041683916555402</v>
@@ -721,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>0.32041683916555402</v>
@@ -738,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>0.32041683916555402</v>
@@ -755,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3">
         <v>0.32041683916555402</v>
@@ -772,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>0.32041683916555402</v>
@@ -789,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3">
         <v>0.32041683916555402</v>
@@ -806,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3">
         <v>0.32041683916555402</v>
@@ -823,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3">
         <v>0.32041683916555402</v>
@@ -840,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3">
         <v>0.32041683916555402</v>
@@ -857,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3">
         <v>0.32041683916555402</v>
@@ -874,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
         <v>0.32041683916555402</v>
@@ -891,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
         <v>0.32041683916555402</v>
@@ -906,5 +914,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>